<commit_message>
Biotech Expansion - Core 업데이트
Co-Authored-By: moonjigi <152117758+moonjigi0723@users.noreply.github.com>

#1837
</commit_message>
<xml_diff>
--- a/Data/Biotech Expansion - Core - 2884018485/1.5/2884018485.xlsx
+++ b/Data/Biotech Expansion - Core - 2884018485/1.5/2884018485.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Biotech Expansion - Core -DO NOT USE-</t>
   </si>
   <si>
-    <t xml:space="preserve">바이오테크 확장팩 - 코어 - 사용하지 마세요</t>
+    <t xml:space="preserve">바이오테크 확장 - 코어 -사용 금지-</t>
   </si>
   <si>
     <t xml:space="preserve">GeneCategoryDef+BTE_Universal.label</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Biotech Expansion - Universal</t>
   </si>
   <si>
-    <t xml:space="preserve">바이오테크 확장팩 - 기본</t>
+    <t xml:space="preserve">바이오테크 확장 - 공용</t>
   </si>
   <si>
     <t xml:space="preserve">GeneDef+BTE_ShearableGene.label</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">SHEARINGCOREGENE</t>
   </si>
   <si>
-    <t xml:space="preserve">털깎기 코어 유전자</t>
+    <t xml:space="preserve">털관련 코어 유전자</t>
   </si>
   <si>
     <t xml:space="preserve">GeneDef+BTE_ShearableGene.description</t>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">Core gene for Biotech Expansion. Do Not Use!</t>
   </si>
   <si>
-    <t xml:space="preserve">바이오테크 확장팩을 위한 코어 유전자입니다. 사용하지 마세요!</t>
+    <t xml:space="preserve">바이오테크 확장을 위한 핵심 유전자. 사용하지 마세요!</t>
   </si>
   <si>
     <t xml:space="preserve">GeneDef+BTE_MilkableGene.label</t>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">MILKCOREGENE</t>
   </si>
   <si>
-    <t xml:space="preserve">밀크 코어 유전자</t>
+    <t xml:space="preserve">착유 코어 유전자</t>
   </si>
   <si>
     <t xml:space="preserve">GeneDef+BTE_MilkableGene.description</t>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">feral might</t>
   </si>
   <si>
-    <t xml:space="preserve">야생의 힘</t>
+    <t xml:space="preserve">야수성</t>
   </si>
   <si>
     <t xml:space="preserve">GeneDef+BTE_FeralMight.description</t>
@@ -133,7 +133,7 @@
     <t xml:space="preserve">Carriers of this gene are instinctual experts at wielding their natural and implanted weapons. If their hands are free, they gain a bonus to melee damage. This stacks along with other melee damage genes.</t>
   </si>
   <si>
-    <t xml:space="preserve">이 유전자의 소유자는 일반적인 무기와 임플란트 무기를 사용하는 데에 본능적인 전문가들입니다. 손이 자유로울 때, 근접 피해량에 보너스를 받습니다. 다른 근접 피해량 유전자와 중첩됩니다.</t>
+    <t xml:space="preserve">이 유전자의 보유자는 타고난 신체를 본능적으로 잘 다루는 전문가입니다. 맨손일 경우 근접 공격력이 증가합니다. 이는 다른 근접 공격력 관련 유전자와 중첩됩니다.</t>
   </si>
   <si>
     <t xml:space="preserve">GeneDef+BTE_Carnivorous.label</t>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">Carriers of this gene are incapable of properly digesting plant based foods. Attempting to do so guarantees food poisoning. Carriers are more accepting of eating raw corpses, however.</t>
   </si>
   <si>
-    <t xml:space="preserve">이 유전자의 소유자는 식물성 음식을 섭취할 수 없습니다. 식물성 음식을 섭취하려고 하는 행동은 식중독을 유발합니다. 대신, 신선한 시체를 섭취하는 것은 허용됩니다.</t>
+    <t xml:space="preserve">이 유전자의 보유자는 식물성 식품을 제대로 소화할 수 없습니다. 섭취할 경우 반드시 식중독에 걸립니다. 하지만 시체를 먹는 것에는 거부감이 적습니다.</t>
   </si>
   <si>
     <t xml:space="preserve">GeneDef+BTE_Herbivorous.label</t>
@@ -181,7 +181,7 @@
     <t xml:space="preserve">Carriers of this gene are incapable of properly digesting meat. Attempting to do so guarantees food poisoning.</t>
   </si>
   <si>
-    <t xml:space="preserve">이 유전자의 소유자는 육류를 섭취할 수 없습니다. 육류를 섭취하려고 하는 행동은 식중독을 유발합니다.</t>
+    <t xml:space="preserve">이 유전자의 보유자는 고기를 제대로 소화할 수 없습니다. 섭취할 경우 반드시 식중독에 걸립니다.</t>
   </si>
   <si>
     <t xml:space="preserve">GeneDef+BTE_BeardlessFurskin.label</t>
@@ -193,7 +193,7 @@
     <t xml:space="preserve">beardless furskin</t>
   </si>
   <si>
-    <t xml:space="preserve">수염 없는 털피부</t>
+    <t xml:space="preserve">대머리 털복숭이</t>
   </si>
   <si>
     <t xml:space="preserve">GeneDef+BTE_BeardlessFurskin.labelShortAdj</t>
@@ -205,7 +205,7 @@
     <t xml:space="preserve">furskinned</t>
   </si>
   <si>
-    <t xml:space="preserve">털난 피부</t>
+    <t xml:space="preserve">변종 털복숭이</t>
   </si>
   <si>
     <t xml:space="preserve">GeneDef+BTE_BeardlessFurskin.description</t>
@@ -217,7 +217,7 @@
     <t xml:space="preserve">Carriers of this gene grow thick fur all over their body, which protects them from cold temperatures. This variant has reduced fur along the facial and head area.</t>
   </si>
   <si>
-    <t xml:space="preserve">이 유전자의 소유자는 몸에 털이 빽빽하게 나, 낮은 기온으로부터 보호받습니다. 이 변이는 머리와 얼굴의 털이 나지 않습니다.</t>
+    <t xml:space="preserve">이 유전자의 보유자는 몸 전체에 두꺼운 털이 자라서 추운 온도로부터 보호합니다. 이 변종은 얼굴과 머리 부분의 털이 적습니다.</t>
   </si>
   <si>
     <t xml:space="preserve">PawnKindDef+BTE_CarniTribal_Penitent.label</t>
@@ -244,7 +244,7 @@
     <t xml:space="preserve">archer</t>
   </si>
   <si>
-    <t xml:space="preserve">궁사</t>
+    <t xml:space="preserve">궁수</t>
   </si>
   <si>
     <t xml:space="preserve">PawnKindDef+BTE_CarniTribal_Warrior.label</t>
@@ -304,7 +304,7 @@
     <t xml:space="preserve">heavy archer</t>
   </si>
   <si>
-    <t xml:space="preserve">장갑 궁사</t>
+    <t xml:space="preserve">강궁수</t>
   </si>
   <si>
     <t xml:space="preserve">PawnKindDef+BTE_CarniTribal_ChiefMelee.label</t>
@@ -316,7 +316,7 @@
     <t xml:space="preserve">berserker chief</t>
   </si>
   <si>
-    <t xml:space="preserve">광전사 대장</t>
+    <t xml:space="preserve">우두머리 광전사</t>
   </si>
   <si>
     <t xml:space="preserve">PawnKindDef+BTE_CarniTribal_ChiefRanged.label</t>
@@ -328,7 +328,7 @@
     <t xml:space="preserve">archer chief</t>
   </si>
   <si>
-    <t xml:space="preserve">궁사 대장</t>
+    <t xml:space="preserve">우두머리 궁사</t>
   </si>
   <si>
     <t xml:space="preserve">PawnKindDef+BTE_CarniTribal_Miner.label</t>
@@ -352,7 +352,7 @@
     <t xml:space="preserve">logger</t>
   </si>
   <si>
-    <t xml:space="preserve">나무꾼</t>
+    <t xml:space="preserve">벌목꾼</t>
   </si>
   <si>
     <t xml:space="preserve">PawnKindDef+BTE_CarniTribal_Farmer.label</t>
@@ -376,7 +376,7 @@
     <t xml:space="preserve">villager</t>
   </si>
   <si>
-    <t xml:space="preserve">마을 사람</t>
+    <t xml:space="preserve">주민</t>
   </si>
   <si>
     <t xml:space="preserve">PawnKindDef+BTE_CarniTribal_Breacher.label</t>
@@ -388,7 +388,7 @@
     <t xml:space="preserve">breacher</t>
   </si>
   <si>
-    <t xml:space="preserve">선봉대</t>
+    <t xml:space="preserve">돌격병</t>
   </si>
 </sst>
 </file>
@@ -675,7 +675,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
+      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.6328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -685,8 +685,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="50.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="26.68"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="8" style="1" width="7.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="40.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16381" min="7" style="1" width="7.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16382" min="16382" style="0" width="9.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16383" min="16383" style="0" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="9.63"/>
   </cols>
   <sheetData>

</xml_diff>